<commit_message>
Added average functions for PHA
</commit_message>
<xml_diff>
--- a/Test Excels/PHA_Crawler_Test_Excel.xlsx
+++ b/Test Excels/PHA_Crawler_Test_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaval\SectionM8-Demo-Fall2025\Test Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A85E7C6-C78A-4B3C-BBB0-29ED3C70E190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7419E5A-43E7-42A9-A9FA-0E7D99ACF1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="123">
   <si>
     <t>pha_code</t>
   </si>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1059,6 +1059,9 @@
       <c r="O3" s="3">
         <v>2914</v>
       </c>
+      <c r="Q3">
+        <v>0.91</v>
+      </c>
       <c r="R3">
         <v>0.11</v>
       </c>
@@ -1076,6 +1079,12 @@
       </c>
       <c r="Y3" s="3">
         <v>2025</v>
+      </c>
+      <c r="Z3">
+        <v>43208.45</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>105</v>
       </c>
       <c r="AJ3" s="3" t="s">
         <v>87</v>

</xml_diff>